<commit_message>
mejore el uso de directorios
</commit_message>
<xml_diff>
--- a/retiros/retiros_puerto.xlsx
+++ b/retiros/retiros_puerto.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,11 +467,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FCIU9139131</t>
+          <t>MSKU9167801</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45174.74791666667</v>
+        <v>45174.6875</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -484,17 +484,17 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>81823</v>
+        <v>82589</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SEKU6214868</t>
+          <t>MSKU8950767</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45174.74791666667</v>
+        <v>45174.69791666666</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -507,17 +507,17 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>83744</v>
+        <v>82566</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CSNU7621463</t>
+          <t>MRKU2590580</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45174.83194444444</v>
+        <v>45174.70833333334</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -530,17 +530,17 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>82429</v>
+        <v>82571</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>TCLU8670727</t>
+          <t>HASU4761072</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45174.84305555555</v>
+        <v>45174.73958333334</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -553,17 +553,17 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>82435</v>
+        <v>82590</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>OOCU7014244</t>
+          <t>MSKU1728038</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45174.84444444445</v>
+        <v>45174.83333333334</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -576,17 +576,17 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>82442</v>
+        <v>82152</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>TRHU8441357</t>
+          <t>FCIU9139131</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45174.84583333333</v>
+        <v>45174.74791666667</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -599,17 +599,17 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>82436</v>
+        <v>81823</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>TRHU6448521</t>
+          <t>SEKU6214868</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45174.35972222222</v>
+        <v>45174.74791666667</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -622,17 +622,17 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>83634</v>
+        <v>83744</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ONEU9126017</t>
+          <t>AMCU9389196</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45174.38194444445</v>
+        <v>45174.75347222222</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -645,17 +645,17 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>83532</v>
+        <v>83961</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>TTNU1032079</t>
+          <t>CSNU7621463</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45174.40277777778</v>
+        <v>45174.83194444444</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -668,17 +668,17 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>83388</v>
+        <v>82429</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>TCNU5127950</t>
+          <t>TCLU8670727</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>45174.45763888889</v>
+        <v>45174.84305555555</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -691,17 +691,17 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>83614</v>
+        <v>82435</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MSMU8707070</t>
+          <t>OOCU7014244</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>45174.46180555555</v>
+        <v>45174.84444444445</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -714,17 +714,17 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>83600</v>
+        <v>82442</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MSMU4853939</t>
+          <t>TRHU8441357</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>45174.46388888889</v>
+        <v>45174.84583333333</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -737,17 +737,17 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>83623</v>
+        <v>82436</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>TGBU4626220</t>
+          <t>TRHU6448521</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>45174.46944444445</v>
+        <v>45174.35972222222</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -760,17 +760,17 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>83617</v>
+        <v>83634</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>FFAU3789894</t>
+          <t>ONEU9126017</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>45174.47291666667</v>
+        <v>45174.38194444445</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -783,17 +783,17 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>83556</v>
+        <v>83532</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MSDU5150894</t>
+          <t>TTNU1032079</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>45174.47638888889</v>
+        <v>45174.40277777778</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -806,17 +806,17 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>83547</v>
+        <v>83388</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>MSDU5203989</t>
+          <t>TCNU5127950</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>45174.48819444444</v>
+        <v>45174.45763888889</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -829,17 +829,17 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>83584</v>
+        <v>83614</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>HMMU6414116</t>
+          <t>MSMU8707070</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>45174.49791666667</v>
+        <v>45174.46180555555</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -852,17 +852,17 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>83601</v>
+        <v>83600</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TTNU8192802</t>
+          <t>MSMU4853939</t>
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>45174.5</v>
+        <v>45174.46388888889</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -875,17 +875,17 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>83300</v>
+        <v>83623</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>MSDU5718794</t>
+          <t>TGBU4626220</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>45174.50416666667</v>
+        <v>45174.46944444445</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -898,17 +898,17 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>83562</v>
+        <v>83617</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>FDCU0614143</t>
+          <t>FFAU3789894</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>45174.50555555556</v>
+        <v>45174.47291666667</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -921,17 +921,17 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>83602</v>
+        <v>83556</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>MSCU5489539</t>
+          <t>MSDU5150894</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>45174.50694444445</v>
+        <v>45174.47638888889</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -944,17 +944,17 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>83615</v>
+        <v>83547</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>TRHU7933584</t>
+          <t>MSDU5203989</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>45174.50972222222</v>
+        <v>45174.48819444444</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -967,17 +967,17 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>83386</v>
+        <v>83584</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>FSCU5732240</t>
+          <t>HMMU6414116</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>45174.5125</v>
+        <v>45174.49791666667</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -990,17 +990,17 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>83895</v>
+        <v>83601</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>NYKU4432188</t>
+          <t>TTNU8192802</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>45174.56944444445</v>
+        <v>45174.5</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1013,17 +1013,17 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>83541</v>
+        <v>83300</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>TRHU5561256</t>
+          <t>MSDU5718794</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>45174.57083333333</v>
+        <v>45174.50416666667</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1036,17 +1036,17 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>83551</v>
+        <v>83562</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>TGBU9243183</t>
+          <t>FDCU0614143</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>45174.57986111111</v>
+        <v>45174.50555555556</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1059,17 +1059,17 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>83558</v>
+        <v>83602</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>BMOU4307044</t>
+          <t>MSCU5489539</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>45174.66944444444</v>
+        <v>45174.50694444445</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1082,17 +1082,17 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>83603</v>
+        <v>83615</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>MSMU7442206</t>
+          <t>TRHU7933584</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>45174.68472222222</v>
+        <v>45174.50972222222</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1105,17 +1105,17 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>83581</v>
+        <v>83386</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CAIU4912615</t>
+          <t>FSCU5732240</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>45174.68611111111</v>
+        <v>45174.5125</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1128,17 +1128,17 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>83280</v>
+        <v>83895</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>MEDU7724633</t>
+          <t>NYKU4432188</t>
         </is>
       </c>
       <c r="B31" s="2" t="n">
-        <v>45174.7125</v>
+        <v>45174.56944444445</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1151,17 +1151,17 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>83542</v>
+        <v>83541</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CAIU8946969</t>
+          <t>TRHU5561256</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>45174.825</v>
+        <v>45174.57083333333</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1174,17 +1174,17 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>83281</v>
+        <v>83551</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>TRIU8090111</t>
+          <t>TGBU9243183</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>45174.82638888889</v>
+        <v>45174.57986111111</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1197,17 +1197,17 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>83894</v>
+        <v>83558</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>NYKU4831249</t>
+          <t>BMOU4307044</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>45174.8875</v>
+        <v>45174.66944444444</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1220,17 +1220,17 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>83563</v>
+        <v>83603</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>TCNU8719167</t>
+          <t>MSMU7442206</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>45174.89583333334</v>
+        <v>45174.68472222222</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1243,17 +1243,17 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>83605</v>
+        <v>83581</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>TTNU8798981</t>
+          <t>CAIU4912615</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>45174.89861111111</v>
+        <v>45174.68611111111</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1266,17 +1266,17 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>83360</v>
+        <v>83280</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>HAMU1257810</t>
+          <t>MEDU7724633</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>45174.35416666666</v>
+        <v>45174.7125</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1289,17 +1289,17 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>83527</v>
+        <v>83542</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>HLBU3363149</t>
+          <t>CAIU8946969</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>45174.375</v>
+        <v>45174.825</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1312,17 +1312,17 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>83530</v>
+        <v>83281</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>PONU7837735</t>
+          <t>TRIU8090111</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>45174.35833333333</v>
+        <v>45174.82638888889</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1335,17 +1335,17 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>83214</v>
+        <v>83894</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>MSKU9591907</t>
+          <t>MEDU1070073</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>45174.36388888889</v>
+        <v>45174.83888888889</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1358,17 +1358,17 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>83136</v>
+        <v>83389</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>MRKU3033146</t>
+          <t>NYKU4831249</t>
         </is>
       </c>
       <c r="B41" s="2" t="n">
-        <v>45174.36805555555</v>
+        <v>45174.8875</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1381,17 +1381,17 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>83230</v>
+        <v>83563</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>MRKU4789354</t>
+          <t>TCNU8719167</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
-        <v>45174.36944444444</v>
+        <v>45174.89583333334</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1404,17 +1404,17 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>83232</v>
+        <v>83605</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>MRKU5748160</t>
+          <t>TTNU8798981</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>45174.37361111111</v>
+        <v>45174.89861111111</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1427,17 +1427,17 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>83181</v>
+        <v>83360</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>MRKU3697000</t>
+          <t>HAMU1257810</t>
         </is>
       </c>
       <c r="B44" s="2" t="n">
-        <v>45174.38958333333</v>
+        <v>45174.35416666666</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1450,17 +1450,17 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>83219</v>
+        <v>83527</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>MSKU1667307</t>
+          <t>HLBU3363149</t>
         </is>
       </c>
       <c r="B45" s="2" t="n">
-        <v>45174.39375</v>
+        <v>45174.375</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1473,17 +1473,17 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>83205</v>
+        <v>83530</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>BEAU5815220</t>
+          <t>PONU7837735</t>
         </is>
       </c>
       <c r="B46" s="2" t="n">
-        <v>45174.39583333334</v>
+        <v>45174.35833333333</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1496,17 +1496,17 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>83160</v>
+        <v>83214</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>MSKU9900903</t>
+          <t>MSKU9591907</t>
         </is>
       </c>
       <c r="B47" s="2" t="n">
-        <v>45174.40208333333</v>
+        <v>45174.36388888889</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1519,17 +1519,17 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>83198</v>
+        <v>83136</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>CIPU5225331</t>
+          <t>MRKU3033146</t>
         </is>
       </c>
       <c r="B48" s="2" t="n">
-        <v>45174.40416666667</v>
+        <v>45174.36805555555</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1542,17 +1542,17 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>83147</v>
+        <v>83230</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>MRKU4002643</t>
+          <t>MRKU4789354</t>
         </is>
       </c>
       <c r="B49" s="2" t="n">
-        <v>45174.40833333333</v>
+        <v>45174.36944444444</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1565,17 +1565,17 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>83192</v>
+        <v>83232</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>HASU4654140</t>
+          <t>MRKU5748160</t>
         </is>
       </c>
       <c r="B50" s="2" t="n">
-        <v>45174.4125</v>
+        <v>45174.37361111111</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1588,17 +1588,17 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>83167</v>
+        <v>83181</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>TCNU2830867</t>
+          <t>MRKU3697000</t>
         </is>
       </c>
       <c r="B51" s="2" t="n">
-        <v>45174.43541666667</v>
+        <v>45174.38958333333</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1611,17 +1611,17 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>83210</v>
+        <v>83219</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>TCKU7626785</t>
+          <t>MSKU1667307</t>
         </is>
       </c>
       <c r="B52" s="2" t="n">
-        <v>45174.44166666667</v>
+        <v>45174.39375</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1634,86 +1634,86 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>83170</v>
+        <v>83205</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>MRKU3125324</t>
+          <t>BEAU5815220</t>
         </is>
       </c>
       <c r="B53" s="2" t="n">
-        <v>45174.37847222222</v>
+        <v>45174.39583333334</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Valparaíso</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>tps</t>
+          <t>sti</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>83764</v>
+        <v>83160</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>TCNU1729815</t>
+          <t>MSKU9900903</t>
         </is>
       </c>
       <c r="B54" s="2" t="n">
-        <v>45174.43472222222</v>
+        <v>45174.40208333333</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Valparaíso</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>tps</t>
+          <t>sti</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>83745</v>
+        <v>83198</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>FCIU4412177</t>
+          <t>CIPU5225331</t>
         </is>
       </c>
       <c r="B55" s="2" t="n">
-        <v>45174.39097222222</v>
+        <v>45174.40416666667</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Valparaíso</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>tps</t>
+          <t>sti</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>83646</v>
+        <v>83147</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>CMAU6555377</t>
+          <t>MRKU4002643</t>
         </is>
       </c>
       <c r="B56" s="2" t="n">
-        <v>45174.52638888889</v>
+        <v>45174.40833333333</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1722,21 +1722,21 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>dpw</t>
+          <t>sti</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>83702</v>
+        <v>83192</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>BEAU5958318</t>
+          <t>HASU4654140</t>
         </is>
       </c>
       <c r="B57" s="2" t="n">
-        <v>45174.52777777778</v>
+        <v>45174.4125</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1745,33 +1745,194 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>dpw</t>
+          <t>sti</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>83701</v>
+        <v>83167</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
+          <t>TCNU2830867</t>
+        </is>
+      </c>
+      <c r="B58" s="2" t="n">
+        <v>45174.43541666667</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>83210</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>TCKU7626785</t>
+        </is>
+      </c>
+      <c r="B59" s="2" t="n">
+        <v>45174.44166666667</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>83170</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>MRKU3125324</t>
+        </is>
+      </c>
+      <c r="B60" s="2" t="n">
+        <v>45174.37847222222</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Valparaíso</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>tps</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>83764</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>TCNU1729815</t>
+        </is>
+      </c>
+      <c r="B61" s="2" t="n">
+        <v>45174.43472222222</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Valparaíso</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>tps</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>83745</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>FCIU4412177</t>
+        </is>
+      </c>
+      <c r="B62" s="2" t="n">
+        <v>45174.39097222222</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Valparaíso</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>tps</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>83646</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>CMAU6555377</t>
+        </is>
+      </c>
+      <c r="B63" s="2" t="n">
+        <v>45174.52638888889</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>dpw</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>83702</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>BEAU5958318</t>
+        </is>
+      </c>
+      <c r="B64" s="2" t="n">
+        <v>45174.52777777778</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>dpw</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>83701</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
           <t>TCNU2751536</t>
         </is>
       </c>
-      <c r="B58" s="2" t="n">
+      <c r="B65" s="2" t="n">
         <v>45174.73541666667</v>
       </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
         <is>
           <t>dpw</t>
         </is>
       </c>
-      <c r="E58" t="n">
+      <c r="E65" t="n">
         <v>83730</v>
       </c>
     </row>

</xml_diff>

<commit_message>
primer commit de development: se agrego un analisis de percentiles a las presentaciones
</commit_message>
<xml_diff>
--- a/retiros/retiros_puerto.xlsx
+++ b/retiros/retiros_puerto.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,11 +467,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MSKU9167801</t>
+          <t>BEAU6161313</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45174.6875</v>
+        <v>45180.58333333334</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -484,17 +484,17 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>82589</v>
+        <v>83512</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MSKU8950767</t>
+          <t>FDCU0099697</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45174.69791666666</v>
+        <v>45180.5875</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -507,17 +507,17 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>82566</v>
+        <v>83464</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MRKU2590580</t>
+          <t>BEAU5580444</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45174.70833333334</v>
+        <v>45180.58888888889</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -530,17 +530,17 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>82571</v>
+        <v>83497</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HASU4761072</t>
+          <t>OOLU9852920</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45174.73958333334</v>
+        <v>45180.59166666667</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -553,17 +553,17 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>82590</v>
+        <v>83460</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MSKU1728038</t>
+          <t>FFAU3095358</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45174.83333333334</v>
+        <v>45180.59305555555</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -576,17 +576,17 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>82152</v>
+        <v>83478</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>FCIU9139131</t>
+          <t>FCIU9905047</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45174.74791666667</v>
+        <v>45180.59444444445</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -599,17 +599,17 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>81823</v>
+        <v>83483</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SEKU6214868</t>
+          <t>TRHU5345278</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45174.74791666667</v>
+        <v>45180.59583333333</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -622,17 +622,17 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>83744</v>
+        <v>83474</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>AMCU9389196</t>
+          <t>OOCU7592495</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45174.75347222222</v>
+        <v>45180.59722222222</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -645,17 +645,17 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>83961</v>
+        <v>83445</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CSNU7621463</t>
+          <t>OOLU9611435</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45174.83194444444</v>
+        <v>45180.60277777778</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -668,17 +668,17 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>82429</v>
+        <v>83328</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>TCLU8670727</t>
+          <t>DRYU9748660</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>45174.84305555555</v>
+        <v>45180.60555555556</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -691,17 +691,17 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>82435</v>
+        <v>83503</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>OOCU7014244</t>
+          <t>OOCU6798373</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>45174.84444444445</v>
+        <v>45180.60833333333</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -714,17 +714,17 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>82442</v>
+        <v>83521</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>TRHU8441357</t>
+          <t>BSIU9567420</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>45174.84583333333</v>
+        <v>45180.67708333334</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -737,17 +737,17 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>82436</v>
+        <v>83329</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>TRHU6448521</t>
+          <t>OOLU9317354</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>45174.35972222222</v>
+        <v>45180.35416666666</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -760,17 +760,17 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>83634</v>
+        <v>83810</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ONEU9126017</t>
+          <t>CSNU6962146</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>45174.38194444445</v>
+        <v>45180.35694444444</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -783,17 +783,17 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>83532</v>
+        <v>84163</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>TTNU1032079</t>
+          <t>CCLU7490909</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>45174.40277777778</v>
+        <v>45180.36111111111</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -806,17 +806,17 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>83388</v>
+        <v>84154</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>TCNU5127950</t>
+          <t>BSIU9411735</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>45174.45763888889</v>
+        <v>45180.36666666667</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -829,17 +829,17 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>83614</v>
+        <v>83790</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>MSMU8707070</t>
+          <t>TGBU7960328</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>45174.46180555555</v>
+        <v>45180.36805555555</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -852,17 +852,17 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>83600</v>
+        <v>83817</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>MSMU4853939</t>
+          <t>TGHU6900440</t>
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>45174.46388888889</v>
+        <v>45180.37222222222</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -875,17 +875,17 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>83623</v>
+        <v>84160</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>TGBU4626220</t>
+          <t>BSIU9405732</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>45174.46944444445</v>
+        <v>45180.37638888889</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -898,17 +898,17 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>83617</v>
+        <v>84159</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>FFAU3789894</t>
+          <t>CSNU6967786</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>45174.47291666667</v>
+        <v>45180.37916666667</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -921,17 +921,17 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>83556</v>
+        <v>84168</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>MSDU5150894</t>
+          <t>OOCU7369938</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>45174.47638888889</v>
+        <v>45180.41597222222</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -944,17 +944,17 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>83547</v>
+        <v>83804</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>MSDU5203989</t>
+          <t>YMLU5445570</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>45174.48819444444</v>
+        <v>45180.42430555556</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -967,17 +967,17 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>83584</v>
+        <v>83845</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>HMMU6414116</t>
+          <t>WHSU2828623</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>45174.49791666667</v>
+        <v>45180.45555555556</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -990,17 +990,17 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>83601</v>
+        <v>83851</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>TTNU8192802</t>
+          <t>YMLU5385491</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>45174.5</v>
+        <v>45180.49444444444</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1013,17 +1013,17 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>83300</v>
+        <v>83854</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MSDU5718794</t>
+          <t>CSNU6436007</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>45174.50416666667</v>
+        <v>45180.55972222222</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1036,17 +1036,17 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>83562</v>
+        <v>83853</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>FDCU0614143</t>
+          <t>DFSU7497211</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>45174.50555555556</v>
+        <v>45180.575</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1059,17 +1059,17 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>83602</v>
+        <v>84166</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>MSCU5489539</t>
+          <t>SEGU4285148</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>45174.50694444445</v>
+        <v>45180.57708333333</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1082,17 +1082,17 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>83615</v>
+        <v>83827</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>TRHU7933584</t>
+          <t>TCNU3051500</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>45174.50972222222</v>
+        <v>45180.59583333333</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1105,155 +1105,155 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>83386</v>
+        <v>83846</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>FSCU5732240</t>
+          <t>TGBU4321848</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>45174.5125</v>
+        <v>45180.42638888889</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Valparaíso</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>sti</t>
+          <t>tps</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>83895</v>
+        <v>83968</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>NYKU4432188</t>
+          <t>TEMU7402244</t>
         </is>
       </c>
       <c r="B31" s="2" t="n">
-        <v>45174.56944444445</v>
+        <v>45180.60625</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Valparaíso</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>sti</t>
+          <t>tps</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>83541</v>
+        <v>81145</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>TRHU5561256</t>
+          <t>UACU4792731</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>45174.57083333333</v>
+        <v>45180.35763888889</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Valparaíso</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>sti</t>
+          <t>tps</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>83551</v>
+        <v>83956</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>TGBU9243183</t>
+          <t>SEGU9377231</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>45174.57986111111</v>
+        <v>45180.36597222222</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Valparaíso</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>sti</t>
+          <t>tps</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>83558</v>
+        <v>83984</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>BMOU4307044</t>
+          <t>UACU4771662</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>45174.66944444444</v>
+        <v>45180.37013888889</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Valparaíso</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>sti</t>
+          <t>tps</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>83603</v>
+        <v>83985</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>MSMU7442206</t>
+          <t>UETU2374486</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>45174.68472222222</v>
+        <v>45180.49513888889</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Valparaíso</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>sti</t>
+          <t>tps</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>83581</v>
+        <v>84116</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CAIU4912615</t>
+          <t>SGRU2126782</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>45174.68611111111</v>
+        <v>45180.3875</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1262,21 +1262,21 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>sti</t>
+          <t>dpw</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>83280</v>
+        <v>84089</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>MEDU7724633</t>
+          <t>TCKU6217083</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>45174.7125</v>
+        <v>45180.46944444445</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1285,21 +1285,21 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>sti</t>
+          <t>dpw</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>83542</v>
+        <v>84057</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>CAIU8946969</t>
+          <t>TRHU4632967</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>45174.825</v>
+        <v>45180.47222222222</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1308,21 +1308,21 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>sti</t>
+          <t>dpw</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>83281</v>
+        <v>84058</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>TRIU8090111</t>
+          <t>TRHU8577723</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>45174.82638888889</v>
+        <v>45180.54444444444</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1331,21 +1331,21 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>sti</t>
+          <t>dpw</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>83894</v>
+        <v>84056</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>MEDU1070073</t>
+          <t>SEGU4756079</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>45174.83888888889</v>
+        <v>45180.58888888889</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1354,586 +1354,11 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>sti</t>
+          <t>dpw</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>83389</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>NYKU4831249</t>
-        </is>
-      </c>
-      <c r="B41" s="2" t="n">
-        <v>45174.8875</v>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E41" t="n">
-        <v>83563</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>TCNU8719167</t>
-        </is>
-      </c>
-      <c r="B42" s="2" t="n">
-        <v>45174.89583333334</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E42" t="n">
-        <v>83605</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>TTNU8798981</t>
-        </is>
-      </c>
-      <c r="B43" s="2" t="n">
-        <v>45174.89861111111</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E43" t="n">
-        <v>83360</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>HAMU1257810</t>
-        </is>
-      </c>
-      <c r="B44" s="2" t="n">
-        <v>45174.35416666666</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E44" t="n">
-        <v>83527</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>HLBU3363149</t>
-        </is>
-      </c>
-      <c r="B45" s="2" t="n">
-        <v>45174.375</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E45" t="n">
-        <v>83530</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>PONU7837735</t>
-        </is>
-      </c>
-      <c r="B46" s="2" t="n">
-        <v>45174.35833333333</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E46" t="n">
-        <v>83214</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>MSKU9591907</t>
-        </is>
-      </c>
-      <c r="B47" s="2" t="n">
-        <v>45174.36388888889</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E47" t="n">
-        <v>83136</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>MRKU3033146</t>
-        </is>
-      </c>
-      <c r="B48" s="2" t="n">
-        <v>45174.36805555555</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E48" t="n">
-        <v>83230</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>MRKU4789354</t>
-        </is>
-      </c>
-      <c r="B49" s="2" t="n">
-        <v>45174.36944444444</v>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E49" t="n">
-        <v>83232</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>MRKU5748160</t>
-        </is>
-      </c>
-      <c r="B50" s="2" t="n">
-        <v>45174.37361111111</v>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E50" t="n">
-        <v>83181</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>MRKU3697000</t>
-        </is>
-      </c>
-      <c r="B51" s="2" t="n">
-        <v>45174.38958333333</v>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E51" t="n">
-        <v>83219</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>MSKU1667307</t>
-        </is>
-      </c>
-      <c r="B52" s="2" t="n">
-        <v>45174.39375</v>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E52" t="n">
-        <v>83205</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>BEAU5815220</t>
-        </is>
-      </c>
-      <c r="B53" s="2" t="n">
-        <v>45174.39583333334</v>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E53" t="n">
-        <v>83160</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>MSKU9900903</t>
-        </is>
-      </c>
-      <c r="B54" s="2" t="n">
-        <v>45174.40208333333</v>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E54" t="n">
-        <v>83198</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>CIPU5225331</t>
-        </is>
-      </c>
-      <c r="B55" s="2" t="n">
-        <v>45174.40416666667</v>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E55" t="n">
-        <v>83147</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>MRKU4002643</t>
-        </is>
-      </c>
-      <c r="B56" s="2" t="n">
-        <v>45174.40833333333</v>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E56" t="n">
-        <v>83192</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>HASU4654140</t>
-        </is>
-      </c>
-      <c r="B57" s="2" t="n">
-        <v>45174.4125</v>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E57" t="n">
-        <v>83167</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>TCNU2830867</t>
-        </is>
-      </c>
-      <c r="B58" s="2" t="n">
-        <v>45174.43541666667</v>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E58" t="n">
-        <v>83210</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>TCKU7626785</t>
-        </is>
-      </c>
-      <c r="B59" s="2" t="n">
-        <v>45174.44166666667</v>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E59" t="n">
-        <v>83170</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>MRKU3125324</t>
-        </is>
-      </c>
-      <c r="B60" s="2" t="n">
-        <v>45174.37847222222</v>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Valparaíso</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>tps</t>
-        </is>
-      </c>
-      <c r="E60" t="n">
-        <v>83764</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>TCNU1729815</t>
-        </is>
-      </c>
-      <c r="B61" s="2" t="n">
-        <v>45174.43472222222</v>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Valparaíso</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>tps</t>
-        </is>
-      </c>
-      <c r="E61" t="n">
-        <v>83745</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>FCIU4412177</t>
-        </is>
-      </c>
-      <c r="B62" s="2" t="n">
-        <v>45174.39097222222</v>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>Valparaíso</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>tps</t>
-        </is>
-      </c>
-      <c r="E62" t="n">
-        <v>83646</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>CMAU6555377</t>
-        </is>
-      </c>
-      <c r="B63" s="2" t="n">
-        <v>45174.52638888889</v>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>dpw</t>
-        </is>
-      </c>
-      <c r="E63" t="n">
-        <v>83702</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>BEAU5958318</t>
-        </is>
-      </c>
-      <c r="B64" s="2" t="n">
-        <v>45174.52777777778</v>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>dpw</t>
-        </is>
-      </c>
-      <c r="E64" t="n">
-        <v>83701</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>TCNU2751536</t>
-        </is>
-      </c>
-      <c r="B65" s="2" t="n">
-        <v>45174.73541666667</v>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>dpw</t>
-        </is>
-      </c>
-      <c r="E65" t="n">
-        <v>83730</v>
+        <v>84014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agrego informacion del tipo de contenedor al modelo
</commit_message>
<xml_diff>
--- a/retiros/retiros_puerto.xlsx
+++ b/retiros/retiros_puerto.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,15 +463,25 @@
           <t>servicios</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>cont_tamano</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>contenedor_peso</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BEAU6161313</t>
+          <t>FSCU8831885</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45180.58333333334</v>
+        <v>45183.55277777778</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -484,17 +494,25 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>83512</v>
+        <v>84175</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>14190</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FDCU0099697</t>
+          <t>CSNU8020560</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45180.5875</v>
+        <v>45183.575</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -507,17 +525,25 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>83464</v>
+        <v>81524</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>11778</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BEAU5580444</t>
+          <t>IMTU9061620</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45180.58888888889</v>
+        <v>45183.59861111111</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -530,17 +556,25 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>83497</v>
+        <v>84208</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>18445</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>OOLU9852920</t>
+          <t>CAXU3191352</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45180.59166666667</v>
+        <v>45183.36388888889</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -553,17 +587,25 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>83460</v>
+        <v>84339</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>26131</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FFAU3095358</t>
+          <t>CAAU6378471</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45180.59305555555</v>
+        <v>45183.43333333333</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -576,17 +618,25 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>83478</v>
+        <v>84125</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>26026</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>FCIU9905047</t>
+          <t>TRHU4096777</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45180.59444444445</v>
+        <v>45183.43472222222</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -599,17 +649,25 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>83483</v>
+        <v>84121</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>26026</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>TRHU5345278</t>
+          <t>HASU4192079</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45180.59583333333</v>
+        <v>45183.43611111111</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -622,17 +680,25 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>83474</v>
+        <v>84338</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>26015</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>OOCU7592495</t>
+          <t>BSIU8053792</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45180.59722222222</v>
+        <v>45183.43888888889</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -645,17 +711,25 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>83445</v>
+        <v>84120</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>26026</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>OOLU9611435</t>
+          <t>HLXU1187217</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45180.60277777778</v>
+        <v>45183.44583333333</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -668,17 +742,25 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>83328</v>
+        <v>84340</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>26089</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>DRYU9748660</t>
+          <t>DFSU7385016</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>45180.60555555556</v>
+        <v>45183.35416666666</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -691,17 +773,25 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>83503</v>
+        <v>83470</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>4635</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>OOCU6798373</t>
+          <t>SEGU6416817</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>45180.60833333333</v>
+        <v>45183.35694444444</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -714,17 +804,25 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>83521</v>
+        <v>83406</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>4635</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BSIU9567420</t>
+          <t>BMOU1594594</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>45180.67708333334</v>
+        <v>45183.41527777778</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -737,17 +835,25 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>83329</v>
+        <v>83524</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>1553</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>OOLU9317354</t>
+          <t>CSNU6901161</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>45180.35416666666</v>
+        <v>45183.42361111111</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -760,17 +866,25 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>83810</v>
+        <v>83477</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>4656</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CSNU6962146</t>
+          <t>FSCU8720454</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>45180.35694444444</v>
+        <v>45183.42777777778</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -783,17 +897,25 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>84163</v>
+        <v>83410</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>4635</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CCLU7490909</t>
+          <t>OOCU6863376</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>45180.36111111111</v>
+        <v>45183.43194444444</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -806,17 +928,25 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>84154</v>
+        <v>83486</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>4656</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BSIU9411735</t>
+          <t>OOCU6738029</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>45180.36666666667</v>
+        <v>45183.43194444444</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -829,17 +959,25 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>83790</v>
+        <v>83394</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>4635</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>TGBU7960328</t>
+          <t>RFCU4013716</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>45180.36805555555</v>
+        <v>45183.43472222222</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -852,17 +990,25 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>83817</v>
+        <v>83421</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>4635</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TGHU6900440</t>
+          <t>TGBU4377180</t>
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>45180.37222222222</v>
+        <v>45183.43611111111</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -875,17 +1021,25 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>84160</v>
+        <v>83482</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>4656</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BSIU9405732</t>
+          <t>MAGU5266174</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>45180.37638888889</v>
+        <v>45183.4375</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -898,17 +1052,25 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>84159</v>
+        <v>83468</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>4635</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CSNU6967786</t>
+          <t>TGBU4750230</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>45180.37916666667</v>
+        <v>45183.43819444445</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -921,17 +1083,25 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>84168</v>
+        <v>83509</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>4659</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>OOCU7369938</t>
+          <t>TCNU1345147</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>45180.41597222222</v>
+        <v>45183.44027777778</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -944,17 +1114,25 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>83804</v>
+        <v>83455</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>4635</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>YMLU5445570</t>
+          <t>FSCU8678694</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>45180.42430555556</v>
+        <v>45183.44305555556</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -967,17 +1145,25 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>83845</v>
+        <v>83510</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>4659</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>WHSU2828623</t>
+          <t>CSNU7204201</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>45180.45555555556</v>
+        <v>45183.44444444445</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -990,17 +1176,25 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>83851</v>
+        <v>83317</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>4696</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>YMLU5385491</t>
+          <t>OOCU8100809</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>45180.49444444444</v>
+        <v>45183.44652777778</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1013,17 +1207,25 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>83854</v>
+        <v>83425</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>4635</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CSNU6436007</t>
+          <t>CSNU8450508</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>45180.55972222222</v>
+        <v>45183.44861111111</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1036,17 +1238,25 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>83853</v>
+        <v>83519</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>4659</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>DFSU7497211</t>
+          <t>FSCU8626670</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>45180.575</v>
+        <v>45183.45</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1059,17 +1269,25 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>84166</v>
+        <v>83454</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>4635</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SEGU4285148</t>
+          <t>BMOU5819786</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>45180.57708333333</v>
+        <v>45183.45069444444</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1082,17 +1300,25 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>83827</v>
+        <v>83491</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>4656</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>TCNU3051500</t>
+          <t>GCXU5635265</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>45180.59583333333</v>
+        <v>45183.45138888889</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1105,155 +1331,211 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>83846</v>
+        <v>83489</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>4656</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>TGBU4321848</t>
+          <t>FFAU3257504</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>45180.42638888889</v>
+        <v>45183.45277777778</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Valparaíso</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>tps</t>
+          <t>sti</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>83968</v>
+        <v>83456</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>4635</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>TEMU7402244</t>
+          <t>OOCU8268449</t>
         </is>
       </c>
       <c r="B31" s="2" t="n">
-        <v>45180.60625</v>
+        <v>45183.45277777778</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Valparaíso</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>tps</t>
+          <t>sti</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>81145</v>
+        <v>83405</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>4635</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>UACU4792731</t>
+          <t>FSCU7092610</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>45180.35763888889</v>
+        <v>45183.45416666667</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Valparaíso</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>tps</t>
+          <t>sti</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>83956</v>
+        <v>83415</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>4635</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SEGU9377231</t>
+          <t>DFSU6928356</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>45180.36597222222</v>
+        <v>45183.45486111111</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Valparaíso</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>tps</t>
+          <t>sti</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>83984</v>
+        <v>83463</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>4635</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>UACU4771662</t>
+          <t>OOCU7221690</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>45180.37013888889</v>
+        <v>45183.45694444444</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Valparaíso</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>tps</t>
+          <t>sti</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>83985</v>
+        <v>83473</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>4656</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>UETU2374486</t>
+          <t>BSIU9586292</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>45180.49513888889</v>
+        <v>45183.45902777778</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Valparaíso</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>tps</t>
+          <t>sti</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>84116</v>
+        <v>83475</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>4656</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>SGRU2126782</t>
+          <t>TCNU1321910</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>45180.3875</v>
+        <v>45183.46111111111</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1262,21 +1544,29 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>dpw</t>
+          <t>sti</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>84089</v>
+        <v>83505</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>4656</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>TCKU6217083</t>
+          <t>OOCU9080380</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>45180.46944444445</v>
+        <v>45183.47152777778</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1285,21 +1575,29 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>dpw</t>
+          <t>sti</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>84057</v>
+        <v>83469</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>4635</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>TRHU4632967</t>
+          <t>CSNU7686762</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>45180.47222222222</v>
+        <v>45183.55416666667</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1308,21 +1606,29 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>dpw</t>
+          <t>sti</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>84058</v>
+        <v>84013</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>9370</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>TRHU8577723</t>
+          <t>OOCU7092930</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>45180.54444444444</v>
+        <v>45183.55555555555</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1331,21 +1637,29 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>dpw</t>
+          <t>sti</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>84056</v>
+        <v>83400</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>4635</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>SEGU4756079</t>
+          <t>DFSU7116980</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>45180.58888888889</v>
+        <v>45183.55694444444</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1354,11 +1668,391 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>83492</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>4656</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>OOLU9824390</t>
+        </is>
+      </c>
+      <c r="B41" s="2" t="n">
+        <v>45183.55833333333</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>83411</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>4635</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>CBHU8982400</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="n">
+        <v>45183.56388888889</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>83440</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>4635</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>FFAU2418667</t>
+        </is>
+      </c>
+      <c r="B43" s="2" t="n">
+        <v>45183.56666666667</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>83487</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>4656</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>CCLU7420666</t>
+        </is>
+      </c>
+      <c r="B44" s="2" t="n">
+        <v>45183.56805555556</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>83409</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>4635</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>FFAU2676661</t>
+        </is>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>45183.56944444445</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>83517</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>4659</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>DFSU6318775</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="n">
+        <v>45183.57083333333</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>83504</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>4656</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>DFSU7664880</t>
+        </is>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>45183.57361111111</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>81416</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>16382</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>FCIU9835470</t>
+        </is>
+      </c>
+      <c r="B48" s="2" t="n">
+        <v>45183.57638888889</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>83476</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>4656</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>CSNU8160509</t>
+        </is>
+      </c>
+      <c r="B49" s="2" t="n">
+        <v>45183.57777777778</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>83321</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>4406</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>OOLU9971365</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="n">
+        <v>45183.57916666667</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>83407</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>4635</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>TEMU9179870</t>
+        </is>
+      </c>
+      <c r="B51" s="2" t="n">
+        <v>45183.39930555555</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Valparaíso</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>tps</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>84295</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>11594</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>TRHU5665862</t>
+        </is>
+      </c>
+      <c r="B52" s="2" t="n">
+        <v>45183.60763888889</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
           <t>dpw</t>
         </is>
       </c>
-      <c r="E40" t="n">
-        <v>84014</v>
+      <c r="E52" t="n">
+        <v>84026</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>22509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agrego estructuras try-except para evitar caida del sistema ante problemas de descarga de retiros
</commit_message>
<xml_diff>
--- a/retiros/retiros_puerto.xlsx
+++ b/retiros/retiros_puerto.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,11 +477,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FSCU8831885</t>
+          <t>EMCU8661262</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45183.55277777778</v>
+        <v>45190.66805555556</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>84175</v>
+        <v>84622</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -502,17 +502,17 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>14190</v>
+        <v>18056</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CSNU8020560</t>
+          <t>TGBU4803264</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45183.575</v>
+        <v>45190.36111111111</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>81524</v>
+        <v>84569</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -533,17 +533,17 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>11778</v>
+        <v>9650</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>IMTU9061620</t>
+          <t>MSMU7320980</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45183.59861111111</v>
+        <v>45190.36458333334</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>84208</v>
+        <v>84564</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -564,17 +564,17 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>18445</v>
+        <v>6410</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CAXU3191352</t>
+          <t>MSMU4077780</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45183.36388888889</v>
+        <v>45190.39444444444</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -587,25 +587,25 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>84339</v>
+        <v>84579</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>40</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>26131</v>
+        <v>7580</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CAAU6378471</t>
+          <t>OTPU6013773</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45183.43333333333</v>
+        <v>45190.39652777778</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -618,7 +618,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>84125</v>
+        <v>84113</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -626,17 +626,17 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>26026</v>
+        <v>6884</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>TRHU4096777</t>
+          <t>MSDU7118926</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45183.43472222222</v>
+        <v>45190.40208333333</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -649,7 +649,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>84121</v>
+        <v>84618</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -657,17 +657,17 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>26026</v>
+        <v>24790</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HASU4192079</t>
+          <t>MSMU6486093</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45183.43611111111</v>
+        <v>45190.40625</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -680,7 +680,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>84338</v>
+        <v>84617</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -688,17 +688,17 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>26015</v>
+        <v>23950</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BSIU8053792</t>
+          <t>TEMU6885960</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45183.43888888889</v>
+        <v>45190.42291666667</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>84120</v>
+        <v>83782</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -719,17 +719,17 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>26026</v>
+        <v>6838</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>HLXU1187217</t>
+          <t>CAAU5524294</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45183.44583333333</v>
+        <v>45190.42708333334</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -742,25 +742,25 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>84340</v>
+        <v>84553</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>40</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>26089</v>
+        <v>11540</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>DFSU7385016</t>
+          <t>TXGU7095080</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>45183.35416666666</v>
+        <v>45190.43333333333</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -773,7 +773,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>83470</v>
+        <v>83778</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -781,17 +781,17 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>4635</v>
+        <v>6614</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>SEGU6416817</t>
+          <t>FCIU8014530</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>45183.35694444444</v>
+        <v>45190.45347222222</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -804,7 +804,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>83406</v>
+        <v>84543</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -812,17 +812,17 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>4635</v>
+        <v>17460</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BMOU1594594</t>
+          <t>BMOU4974197</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>45183.41527777778</v>
+        <v>45190.45902777778</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -835,25 +835,25 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>83524</v>
+        <v>84482</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>40</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>1553</v>
+        <v>25984</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CSNU6901161</t>
+          <t>GCXU5433372</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>45183.42361111111</v>
+        <v>45190.46805555555</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -866,7 +866,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>83477</v>
+        <v>83355</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -874,17 +874,17 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>4656</v>
+        <v>17924</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>FSCU8720454</t>
+          <t>MSMU8604718</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>45183.42777777778</v>
+        <v>45190.46944444445</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>83410</v>
+        <v>84591</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -905,17 +905,17 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>4635</v>
+        <v>4122</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>OOCU6863376</t>
+          <t>TCNU2401287</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>45183.43194444444</v>
+        <v>45190.49305555555</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>83486</v>
+        <v>84605</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -936,17 +936,17 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>4656</v>
+        <v>8490</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>OOCU6738029</t>
+          <t>DRYU9712610</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>45183.43194444444</v>
+        <v>45190.55</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -959,7 +959,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>83394</v>
+        <v>84320</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -967,17 +967,17 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>4635</v>
+        <v>7172</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>RFCU4013716</t>
+          <t>MSMU5374972</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>45183.43472222222</v>
+        <v>45190.56597222222</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -990,7 +990,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>83421</v>
+        <v>84748</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -998,17 +998,17 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>4635</v>
+        <v>11850</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TGBU4377180</t>
+          <t>FANU3213182</t>
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>45183.43611111111</v>
+        <v>45190.58680555555</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1021,7 +1021,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>83482</v>
+        <v>83777</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1029,17 +1029,17 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>4656</v>
+        <v>6541</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>MAGU5266174</t>
+          <t>UACU5658157</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>45183.4375</v>
+        <v>45190.59513888889</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>83468</v>
+        <v>83781</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1060,17 +1060,17 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>4635</v>
+        <v>6506</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TGBU4750230</t>
+          <t>MEDU8746426</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>45183.43819444445</v>
+        <v>45190.6</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1083,7 +1083,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>83509</v>
+        <v>84538</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1091,17 +1091,17 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>4659</v>
+        <v>8360</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>TCNU1345147</t>
+          <t>BEAU4594546</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>45183.44027777778</v>
+        <v>45190.68055555555</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1114,7 +1114,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>83455</v>
+        <v>84585</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1122,17 +1122,17 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>4635</v>
+        <v>15490</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>FSCU8678694</t>
+          <t>TRHU6635923</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>45183.44305555556</v>
+        <v>45190.71666666667</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1145,7 +1145,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>83510</v>
+        <v>84582</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1153,17 +1153,17 @@
         </is>
       </c>
       <c r="G23" t="n">
-        <v>4659</v>
+        <v>10781</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CSNU7204201</t>
+          <t>FCIU8957811</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>45183.44444444445</v>
+        <v>45190.73055555556</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1176,7 +1176,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>83317</v>
+        <v>84557</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1184,17 +1184,17 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>4696</v>
+        <v>15120</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>OOCU8100809</t>
+          <t>SEKU6065152</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>45183.44652777778</v>
+        <v>45190.73958333334</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1207,7 +1207,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>83425</v>
+        <v>83776</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1215,17 +1215,17 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>4635</v>
+        <v>6445</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CSNU8450508</t>
+          <t>TEMU6575570</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>45183.44861111111</v>
+        <v>45190.74444444444</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1238,7 +1238,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>83519</v>
+        <v>84612</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1246,17 +1246,17 @@
         </is>
       </c>
       <c r="G26" t="n">
-        <v>4659</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>FSCU8626670</t>
+          <t>HLBU9129689</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>45183.45</v>
+        <v>45190.75416666667</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1269,7 +1269,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>83454</v>
+        <v>84570</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1277,17 +1277,17 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>4635</v>
+        <v>9340</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>BMOU5819786</t>
+          <t>ONEU0291710</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>45183.45069444444</v>
+        <v>45190.75972222222</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>83491</v>
+        <v>84359</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1308,17 +1308,17 @@
         </is>
       </c>
       <c r="G28" t="n">
-        <v>4656</v>
+        <v>18040</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>GCXU5635265</t>
+          <t>MSMU4374469</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>45183.45138888889</v>
+        <v>45190.77083333334</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1331,7 +1331,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>83489</v>
+        <v>84292</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1339,17 +1339,17 @@
         </is>
       </c>
       <c r="G29" t="n">
-        <v>4656</v>
+        <v>21168</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>FFAU3257504</t>
+          <t>FSCU8932751</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>45183.45277777778</v>
+        <v>45190.85</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1362,7 +1362,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>83456</v>
+        <v>84602</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1370,17 +1370,17 @@
         </is>
       </c>
       <c r="G30" t="n">
-        <v>4635</v>
+        <v>11400</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>OOCU8268449</t>
+          <t>NYKU4953870</t>
         </is>
       </c>
       <c r="B31" s="2" t="n">
-        <v>45183.45277777778</v>
+        <v>45190.86944444444</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1393,7 +1393,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>83405</v>
+        <v>84560</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1401,17 +1401,17 @@
         </is>
       </c>
       <c r="G31" t="n">
-        <v>4635</v>
+        <v>12960</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>FSCU7092610</t>
+          <t>MSMU8382014</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>45183.45416666667</v>
+        <v>45190.8875</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1424,7 +1424,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>83415</v>
+        <v>84772</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1432,17 +1432,17 @@
         </is>
       </c>
       <c r="G32" t="n">
-        <v>4635</v>
+        <v>9800</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>DFSU6928356</t>
+          <t>TGHU9290269</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>45183.45486111111</v>
+        <v>45190.88888888889</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1455,7 +1455,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>83463</v>
+        <v>84293</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1463,17 +1463,17 @@
         </is>
       </c>
       <c r="G33" t="n">
-        <v>4635</v>
+        <v>11708</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>OOCU7221690</t>
+          <t>BEAU4242627</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>45183.45694444444</v>
+        <v>45190.88888888889</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1486,7 +1486,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>83473</v>
+        <v>84567</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1494,17 +1494,17 @@
         </is>
       </c>
       <c r="G34" t="n">
-        <v>4656</v>
+        <v>11790</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>BSIU9586292</t>
+          <t>HLBU9450174</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>45183.45902777778</v>
+        <v>45190.89444444444</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>83475</v>
+        <v>84571</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1525,17 +1525,17 @@
         </is>
       </c>
       <c r="G35" t="n">
-        <v>4656</v>
+        <v>9430</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>TCNU1321910</t>
+          <t>MOTU1416810</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>45183.46111111111</v>
+        <v>45190.89861111111</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1548,7 +1548,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>83505</v>
+        <v>84555</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -1556,17 +1556,17 @@
         </is>
       </c>
       <c r="G36" t="n">
-        <v>4656</v>
+        <v>24712</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>OOCU9080380</t>
+          <t>FFAU4140791</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>45183.47152777778</v>
+        <v>45190.90833333333</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1579,7 +1579,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>83469</v>
+        <v>84550</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1587,17 +1587,17 @@
         </is>
       </c>
       <c r="G37" t="n">
-        <v>4635</v>
+        <v>23350</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>CSNU7686762</t>
+          <t>MSKU9327258</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>45183.55416666667</v>
+        <v>45190.36666666667</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1610,7 +1610,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>84013</v>
+        <v>84750</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1618,17 +1618,17 @@
         </is>
       </c>
       <c r="G38" t="n">
-        <v>9370</v>
+        <v>9438</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>OOCU7092930</t>
+          <t>MSKU9941841</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>45183.55555555555</v>
+        <v>45190.39166666667</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1641,7 +1641,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>83400</v>
+        <v>84699</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -1649,30 +1649,30 @@
         </is>
       </c>
       <c r="G39" t="n">
-        <v>4635</v>
+        <v>15120</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>DFSU7116980</t>
+          <t>SZLU9703244</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>45183.55694444444</v>
+        <v>45190.56875</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Valparaíso</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>sti</t>
+          <t>tps</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>83492</v>
+        <v>84749</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -1680,30 +1680,30 @@
         </is>
       </c>
       <c r="G40" t="n">
-        <v>4656</v>
+        <v>7224</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>OOLU9824390</t>
+          <t>FANU1994717</t>
         </is>
       </c>
       <c r="B41" s="2" t="n">
-        <v>45183.55833333333</v>
+        <v>45190.60625</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Valparaíso</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>sti</t>
+          <t>tps</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>83411</v>
+        <v>84529</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -1711,30 +1711,30 @@
         </is>
       </c>
       <c r="G41" t="n">
-        <v>4635</v>
+        <v>5109</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CBHU8982400</t>
+          <t>SEKU6412800</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
-        <v>45183.56388888889</v>
+        <v>45190.61666666667</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Valparaíso</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>sti</t>
+          <t>tps</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>83440</v>
+        <v>84527</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -1742,317 +1742,38 @@
         </is>
       </c>
       <c r="G42" t="n">
-        <v>4635</v>
+        <v>5578</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>FFAU2418667</t>
+          <t>MEDU1136289</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>45183.56666666667</v>
+        <v>45190.66597222222</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Valparaíso</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>sti</t>
+          <t>tps</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>83487</v>
+        <v>84751</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>20</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>4656</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>CCLU7420666</t>
-        </is>
-      </c>
-      <c r="B44" s="2" t="n">
-        <v>45183.56805555556</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E44" t="n">
-        <v>83409</v>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="G44" t="n">
-        <v>4635</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>FFAU2676661</t>
-        </is>
-      </c>
-      <c r="B45" s="2" t="n">
-        <v>45183.56944444445</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E45" t="n">
-        <v>83517</v>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="G45" t="n">
-        <v>4659</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>DFSU6318775</t>
-        </is>
-      </c>
-      <c r="B46" s="2" t="n">
-        <v>45183.57083333333</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E46" t="n">
-        <v>83504</v>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="G46" t="n">
-        <v>4656</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>DFSU7664880</t>
-        </is>
-      </c>
-      <c r="B47" s="2" t="n">
-        <v>45183.57361111111</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E47" t="n">
-        <v>81416</v>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="G47" t="n">
-        <v>16382</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>FCIU9835470</t>
-        </is>
-      </c>
-      <c r="B48" s="2" t="n">
-        <v>45183.57638888889</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E48" t="n">
-        <v>83476</v>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="G48" t="n">
-        <v>4656</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>CSNU8160509</t>
-        </is>
-      </c>
-      <c r="B49" s="2" t="n">
-        <v>45183.57777777778</v>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E49" t="n">
-        <v>83321</v>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="G49" t="n">
-        <v>4406</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>OOLU9971365</t>
-        </is>
-      </c>
-      <c r="B50" s="2" t="n">
-        <v>45183.57916666667</v>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="E50" t="n">
-        <v>83407</v>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="G50" t="n">
-        <v>4635</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>TEMU9179870</t>
-        </is>
-      </c>
-      <c r="B51" s="2" t="n">
-        <v>45183.39930555555</v>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Valparaíso</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>tps</t>
-        </is>
-      </c>
-      <c r="E51" t="n">
-        <v>84295</v>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="G51" t="n">
-        <v>11594</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>TRHU5665862</t>
-        </is>
-      </c>
-      <c r="B52" s="2" t="n">
-        <v>45183.60763888889</v>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>San Antonio</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>dpw</t>
-        </is>
-      </c>
-      <c r="E52" t="n">
-        <v>84026</v>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="G52" t="n">
-        <v>22509</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mensaje descriptivo del commit
</commit_message>
<xml_diff>
--- a/retiros/retiros_puerto.xlsx
+++ b/retiros/retiros_puerto.xlsx
@@ -1,66 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>contenedor</t>
-  </si>
-  <si>
-    <t>fecha</t>
-  </si>
-  <si>
-    <t>comuna</t>
-  </si>
-  <si>
-    <t>empresa</t>
-  </si>
-  <si>
-    <t>servicios</t>
-  </si>
-  <si>
-    <t>cont_tamano</t>
-  </si>
-  <si>
-    <t>contenedor_peso</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -75,35 +49,94 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -391,37 +424,336 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>contenedor</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>fecha</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>comuna</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>empresa</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>servicios</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>cont_tamano</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>contenedor_peso</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CMAU3469064</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>45362.35416666666</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>94936</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>25840</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CMAU3076811</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>45362.36319444444</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>95582</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>24922</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CSNU7587414</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>45362.56736111111</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>94204</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>13824</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>OOCU7647638</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>45362.59861111111</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>94207</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>7361</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CSNU7711844</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>45362.60069444445</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>94202</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>5849</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TCNU3455020</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>45362.60277777778</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>95587</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>2670</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>EMCU8636207</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>45362.47916666666</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>94720</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>13800</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>TEMU6356695</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>45362.56319444445</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>94740</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>20860</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>CSNU7275910</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>45362.57708333333</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>San Antonio</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>sti</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>94732</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>12060</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modelo de factibilidad implementado
</commit_message>
<xml_diff>
--- a/retiros/retiros_puerto.xlsx
+++ b/retiros/retiros_puerto.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\modelo_asignacion\retiros\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A1F3D7-C863-4F71-B080-53CDD7494709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -91,11 +97,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,13 +165,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -203,7 +217,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -237,6 +251,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -271,9 +286,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -446,14 +462,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,12 +500,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <v>45448.72361111111</v>
+        <v>45448.723611111112</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -505,12 +526,12 @@
         <v>323756</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2">
-        <v>45448.74166666667</v>
+        <v>45448.741666666669</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -531,12 +552,12 @@
         <v>324594</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2">
-        <v>45448.74861111111</v>
+        <v>45448.748611111107</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -557,7 +578,7 @@
         <v>324832</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -583,7 +604,7 @@
         <v>324370</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -609,12 +630,12 @@
         <v>324202</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="2">
-        <v>45448.75694444445</v>
+        <v>45448.756944444453</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -635,12 +656,12 @@
         <v>324256</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2">
-        <v>45448.75833333333</v>
+        <v>45448.758333333331</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -661,12 +682,12 @@
         <v>324262</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2">
-        <v>45448.77083333334</v>
+        <v>45448.770833333343</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -687,12 +708,12 @@
         <v>324274</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2">
-        <v>45448.775</v>
+        <v>45448.775000000001</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -713,12 +734,12 @@
         <v>324220</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2">
-        <v>45448.78611111111</v>
+        <v>45448.786111111112</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -739,12 +760,12 @@
         <v>323985</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="2">
-        <v>45448.86527777778</v>
+        <v>45448.865277777782</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
@@ -765,12 +786,12 @@
         <v>323759</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="2">
-        <v>45448.92361111111</v>
+        <v>45448.923611111109</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>

</xml_diff>